<commit_message>
18-04-24 | 5:29 PM
</commit_message>
<xml_diff>
--- a/leads_export.xlsx
+++ b/leads_export.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -634,6 +634,398 @@
         <v>45399</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Prasath</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>9876543210</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Inlingua</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Language Center</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Tambaram</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Recurring</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>CRM</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>100000</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>45399</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>45423</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Vignesh</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>prsath@gmail.com</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Call Back</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>45401</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>45399</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Nithya</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9876543210</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Test Company</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Madipakkam</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Recurring</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>45399</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>45416</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Vignesh</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>test@abcd.com</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Do Not Disturb</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>45416</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="V4" s="1" t="n">
+        <v>45400</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Nithya</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>9789513442</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SMK</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Politics</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Guindy</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>One Time</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>SMM</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>45400</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>45404</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nithya@gmail.com</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>abcd</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
+      </c>
+      <c r="S5" s="1" t="n">
+        <v>45396</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="V5" s="1" t="n">
+        <v>45400</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Vino</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>9456239864</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Abc</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Digital marketing</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Velachery</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>One Time</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>CRM</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>20000</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>45400</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>45411</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Google</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Vino@gmail.com</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>cds</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>45405</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="V6" s="1" t="n">
+        <v>45400</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update 31-may-24 | 6:53 PM
</commit_message>
<xml_diff>
--- a/leads_export.xlsx
+++ b/leads_export.xlsx
@@ -467,57 +467,57 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Amount</t>
+          <t>Proposal Amount</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
+          <t>Finally Budget</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>End of Date</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Mail ID</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Additional Remarks</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Call Back Comments</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Call Back</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>Is Customer</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>Created Date</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>End of Date</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Lead Name</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Mail ID</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Comment</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>Remarks</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>Follow Up</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
@@ -539,25 +539,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nithya</t>
+          <t>Vignesh</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9789513442</v>
+        <v>23456789</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SMK</t>
+          <t>Revaa</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Politics</t>
+          <t>Didital Marketing</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Guindy</t>
+          <t>America</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -572,95 +572,93 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>SMM</t>
+          <t>Branding</t>
         </is>
       </c>
       <c r="I2" t="n">
         <v>10000</v>
       </c>
-      <c r="J2" t="b">
+      <c r="J2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>45451</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>vignesh123@gmail.com</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Fresh</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Nothin 2</t>
+        </is>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>45444</v>
+      </c>
+      <c r="R2" t="b">
         <v>0</v>
       </c>
-      <c r="K2" s="1" t="n">
-        <v>45439</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>45404</v>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Chrome</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>nithya@gmail.com</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>abcd</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Nothing</t>
-        </is>
-      </c>
       <c r="S2" s="1" t="n">
-        <v>45396</v>
+        <v>45442</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>vignesh</t>
+          <t>admin</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>vignesh</t>
+          <t>admin</t>
         </is>
       </c>
       <c r="V2" s="1" t="n">
-        <v>45439</v>
+        <v>45442</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Vino</t>
+          <t>Nithya</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9456239864</v>
+        <v>9876543210</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Abc</t>
+          <t>Google</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Digital marketing</t>
+          <t>Product Company</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Velachery</t>
+          <t>America</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Chennai</t>
+          <t>Madhurai</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -670,164 +668,160 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>CRM</t>
+          <t>Branding, Design, SMM</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>20000</v>
-      </c>
-      <c r="J3" t="b">
+        <v>2000</v>
+      </c>
+      <c r="J3" t="n">
+        <v>3000</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>45458</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nithya@gmail.com</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Fresh</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Nothing 1</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Nothing 2</t>
+        </is>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>45451</v>
+      </c>
+      <c r="R3" t="b">
         <v>0</v>
       </c>
-      <c r="K3" s="1" t="n">
-        <v>45439</v>
-      </c>
-      <c r="L3" s="1" t="n">
-        <v>45411</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Google</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Vino@gmail.com</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>cds</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="S3" s="1" t="n">
-        <v>45405</v>
+        <v>45442</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>vignesh</t>
+          <t>admin</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>vignesh</t>
+          <t>admin</t>
         </is>
       </c>
       <c r="V3" s="1" t="n">
-        <v>45439</v>
+        <v>45442</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Liya</t>
+          <t>Ram text</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9123786543</v>
+        <v>987654321000</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>BPO</t>
+          <t>Global</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>software</t>
+          <t>Product Company</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Tamabaram</t>
+          <t>America</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Chennai</t>
+          <t>Madhurai</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>One Time</t>
+          <t>Recurring</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Design</t>
+          <t>Branding</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>5000</v>
-      </c>
-      <c r="J4" t="b">
+        <v>88888</v>
+      </c>
+      <c r="J4" t="n">
+        <v>99999</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>45354</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>test@gmail.com</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Do Not Disturb</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Nothing test 2</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Nothing test</t>
+        </is>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>45354</v>
+      </c>
+      <c r="R4" t="b">
         <v>0</v>
       </c>
-      <c r="K4" s="1" t="n">
-        <v>45439</v>
-      </c>
-      <c r="L4" s="1" t="n">
-        <v>45412</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Google</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>liya@gmail.com</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>mlklk</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>sharf</t>
-        </is>
-      </c>
       <c r="S4" s="1" t="n">
-        <v>45412</v>
+        <v>45442</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>vignesh</t>
+          <t>admin</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>vignesh</t>
+          <t>admin</t>
         </is>
       </c>
       <c r="V4" s="1" t="n">
-        <v>45439</v>
+        <v>45442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
31-05-24 | 7:52 pm
</commit_message>
<xml_diff>
--- a/leads_export.xlsx
+++ b/leads_export.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +447,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Country</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -822,6 +822,198 @@
       </c>
       <c r="V4" s="1" t="n">
         <v>45442</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Example Corp</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Product Company</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>One Time</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Google Adds, Marketing</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J5" t="n">
+        <v>45000</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>45443</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>johndoe@example.com</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Fresh</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Initial contact made</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Follow up next week</t>
+        </is>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>45443</v>
+      </c>
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <v>45443</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="V5" s="1" t="n">
+        <v>45443</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Example Corp</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Product Company</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>One Time</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>SMM</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J6" t="n">
+        <v>45000</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>45443</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>johndoe@example.com</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Fresh</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Initial contact made</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Follow up next week</t>
+        </is>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>45443</v>
+      </c>
+      <c r="R6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>45443</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="V6" s="1" t="n">
+        <v>45443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>